<commit_message>
Remove parameters, update example file
remove all the parameters such as setFinParameters since they are no longer needed. Created new excel file with rocket data that is used to fill the new excel file
</commit_message>
<xml_diff>
--- a/MBSExample.xlsx
+++ b/MBSExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\Code\Gatech\RocketClub\AutoRASAero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B647402-B471-4F4B-9135-744E713F4BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E171A2FF-A29A-4A3B-A704-6762F4887D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8100" yWindow="1650" windowWidth="16200" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Run" sheetId="12" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Booster Root Chord</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>blue'</t>
+  </si>
+  <si>
+    <t>Von Karman Ogive</t>
+  </si>
+  <si>
+    <t>Black</t>
   </si>
 </sst>
 </file>
@@ -557,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2BA41CF-4655-44D2-81BA-3AB1895A7CCD}">
   <dimension ref="A1:AC1120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,91 +1125,91 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
+        <v>34.5</v>
+      </c>
+      <c r="B7">
+        <v>6.17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="B7">
-        <v>500</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7">
-        <v>50</v>
-      </c>
-      <c r="E7">
-        <v>60</v>
+      <c r="E7" t="s">
+        <v>33</v>
       </c>
       <c r="F7">
-        <v>1000</v>
+        <v>17</v>
       </c>
       <c r="G7">
-        <v>10</v>
-      </c>
-      <c r="H7">
-        <v>20</v>
+        <v>6.17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
       </c>
       <c r="I7">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="J7">
-        <v>40</v>
+        <v>6.17</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="L7">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="M7">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="N7">
-        <v>100</v>
+        <v>9</v>
       </c>
       <c r="O7">
-        <v>200</v>
+        <v>5</v>
       </c>
       <c r="P7">
-        <v>300</v>
+        <v>0.5</v>
       </c>
       <c r="Q7">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="R7">
-        <v>20</v>
+        <v>80.5</v>
       </c>
       <c r="S7">
-        <v>30</v>
+        <v>6.17</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="U7">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="V7">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="W7">
-        <v>230</v>
+        <v>9</v>
       </c>
       <c r="X7">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="Y7">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="Z7">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="AA7">
-        <v>30000</v>
+        <v>2050</v>
       </c>
       <c r="AB7">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="AC7">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modify Example.py to iterate a dict. Modify mbsEditor to accept a dict
also make minor fixes such as moving mbsEditor to automation
</commit_message>
<xml_diff>
--- a/MBSExample.xlsx
+++ b/MBSExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\Code\Gatech\RocketClub\AutoRASAero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E171A2FF-A29A-4A3B-A704-6762F4887D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E58829-999E-43F2-8871-8C8BB6C81555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="1650" windowWidth="16200" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Run" sheetId="12" r:id="rId1"/>
@@ -59,54 +59,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
-    <t>Booster Root Chord</t>
-  </si>
-  <si>
-    <t>Booster Span</t>
-  </si>
-  <si>
-    <t>Booster Tip Chord</t>
-  </si>
-  <si>
-    <t>Booster Sweep</t>
-  </si>
-  <si>
-    <t>Sustainer Root Chord</t>
-  </si>
-  <si>
-    <t>Sustainer Span</t>
-  </si>
-  <si>
-    <t>Sustainer Tip Chord</t>
-  </si>
-  <si>
-    <t>Sustainer Sweep</t>
-  </si>
-  <si>
-    <t>Ignition Delay</t>
-  </si>
-  <si>
-    <t>boosterStartStability</t>
-  </si>
-  <si>
-    <t>boosterEndStability</t>
-  </si>
-  <si>
-    <t>sustainerStartStability</t>
-  </si>
-  <si>
-    <t>sustainerMaxStability</t>
-  </si>
-  <si>
-    <t>globalMinStability</t>
-  </si>
-  <si>
-    <t>globalMaxStability</t>
-  </si>
-  <si>
-    <t>apogee</t>
-  </si>
-  <si>
     <t>noseConeLength</t>
   </si>
   <si>
@@ -119,39 +71,6 @@
     <t>red'</t>
   </si>
   <si>
-    <t>apogee2</t>
-  </si>
-  <si>
-    <t>apogee3</t>
-  </si>
-  <si>
-    <t>apogee4</t>
-  </si>
-  <si>
-    <t>apogee5</t>
-  </si>
-  <si>
-    <t>apogee6</t>
-  </si>
-  <si>
-    <t>apogee7</t>
-  </si>
-  <si>
-    <t>apogee8</t>
-  </si>
-  <si>
-    <t>apogee9</t>
-  </si>
-  <si>
-    <t>apogee10</t>
-  </si>
-  <si>
-    <t>apogee11</t>
-  </si>
-  <si>
-    <t>apogee12</t>
-  </si>
-  <si>
     <t>blue'</t>
   </si>
   <si>
@@ -159,6 +78,87 @@
   </si>
   <si>
     <t>Black</t>
+  </si>
+  <si>
+    <t>noseConeShape</t>
+  </si>
+  <si>
+    <t>noseConeBluntRadius</t>
+  </si>
+  <si>
+    <t>noseConeColor</t>
+  </si>
+  <si>
+    <t>bodyTubeLength</t>
+  </si>
+  <si>
+    <t>bodyTubeDiameter</t>
+  </si>
+  <si>
+    <t>bodyTubeColor</t>
+  </si>
+  <si>
+    <t>bodyTubeLength2</t>
+  </si>
+  <si>
+    <t>bodyTubeDiameter2</t>
+  </si>
+  <si>
+    <t>bodyTubeColor2</t>
+  </si>
+  <si>
+    <t>finChord</t>
+  </si>
+  <si>
+    <t>finSpan</t>
+  </si>
+  <si>
+    <t>finSweepDistance</t>
+  </si>
+  <si>
+    <t>finTipChord</t>
+  </si>
+  <si>
+    <t>finThickness</t>
+  </si>
+  <si>
+    <t>finLocation</t>
+  </si>
+  <si>
+    <t>boosterLength</t>
+  </si>
+  <si>
+    <t>boosterDiameter</t>
+  </si>
+  <si>
+    <t>boosterColor</t>
+  </si>
+  <si>
+    <t>finChord2</t>
+  </si>
+  <si>
+    <t>finSpan2</t>
+  </si>
+  <si>
+    <t>finSweepDistance2</t>
+  </si>
+  <si>
+    <t>finTipChord2</t>
+  </si>
+  <si>
+    <t>finThickness2</t>
+  </si>
+  <si>
+    <t>finLocation2</t>
+  </si>
+  <si>
+    <t>altitude</t>
+  </si>
+  <si>
+    <t>rodLength</t>
+  </si>
+  <si>
+    <t>windSpeed</t>
   </si>
 </sst>
 </file>
@@ -266,33 +266,33 @@
   <tableColumns count="29">
     <tableColumn id="1" xr3:uid="{1C5986BD-78F5-442C-A447-E7240EFA4A7F}" uniqueName="1" name="noseConeLength" queryTableFieldId="1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{5A954700-8423-4075-A3A0-7CB57BCB7B71}" uniqueName="2" name="noseConeDiameter" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{FB56DFA2-C792-4CE4-B02B-87EFC9B85F6B}" uniqueName="3" name="Booster Root Chord" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{06131C04-BA24-4F0D-AF3B-724D17016671}" uniqueName="4" name="Booster Span" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{6915BD82-BDC1-41D7-B8A3-302481659DA8}" uniqueName="5" name="Booster Tip Chord" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{F38FA88D-02E0-40D5-AC63-CB0CE515693C}" uniqueName="6" name="Booster Sweep" queryTableFieldId="6"/>
-    <tableColumn id="7" xr3:uid="{C521ED2F-1FC3-4DAB-A9F9-BC51B6DF880D}" uniqueName="7" name="Sustainer Root Chord" queryTableFieldId="7"/>
-    <tableColumn id="8" xr3:uid="{DF644A37-CA42-4F6D-B514-E2DE3DF02CA8}" uniqueName="8" name="Sustainer Span" queryTableFieldId="8"/>
-    <tableColumn id="9" xr3:uid="{D1CA3669-944B-4A99-BC39-6B262233B95C}" uniqueName="9" name="Sustainer Tip Chord" queryTableFieldId="9"/>
-    <tableColumn id="10" xr3:uid="{71E57123-8652-4666-BC1D-F74808687DED}" uniqueName="10" name="Sustainer Sweep" queryTableFieldId="10"/>
-    <tableColumn id="11" xr3:uid="{9CD28011-0BDA-4F24-A0C9-6B11B5373006}" uniqueName="11" name="Ignition Delay" queryTableFieldId="11"/>
-    <tableColumn id="12" xr3:uid="{BA15E9C3-B4CD-4D2B-A5CE-19441D50A3B0}" uniqueName="12" name="boosterStartStability" queryTableFieldId="12"/>
-    <tableColumn id="13" xr3:uid="{41E8443E-1025-4CA7-942D-DB72C9332E20}" uniqueName="13" name="boosterEndStability" queryTableFieldId="13"/>
-    <tableColumn id="14" xr3:uid="{1C88E467-9E1D-4275-BCD3-A4F086870034}" uniqueName="14" name="sustainerStartStability" queryTableFieldId="14"/>
-    <tableColumn id="15" xr3:uid="{A0A7254A-3F92-44E4-BB66-F7C8FD4E4B96}" uniqueName="15" name="sustainerMaxStability" queryTableFieldId="15"/>
-    <tableColumn id="16" xr3:uid="{DA3581A1-3DE9-48D5-9865-AA84BAD78A3C}" uniqueName="16" name="globalMinStability" queryTableFieldId="16"/>
-    <tableColumn id="17" xr3:uid="{7AACB600-B520-4E15-AF33-7B556520FAD1}" uniqueName="17" name="globalMaxStability" queryTableFieldId="17"/>
-    <tableColumn id="18" xr3:uid="{451CDA72-0A69-401E-88DE-FC3AD6E843ED}" uniqueName="18" name="apogee" queryTableFieldId="18"/>
-    <tableColumn id="19" xr3:uid="{9D25066F-609B-46D0-95FD-6CA21A9EEA50}" uniqueName="19" name="apogee2" queryTableFieldId="19"/>
-    <tableColumn id="20" xr3:uid="{1538BFC0-D7C7-4A93-B848-A7F817FE47B3}" uniqueName="20" name="apogee3" queryTableFieldId="20"/>
-    <tableColumn id="21" xr3:uid="{E2FE5987-0CDC-4B54-B449-7EFEC5EE712B}" uniqueName="21" name="apogee4" queryTableFieldId="21"/>
-    <tableColumn id="22" xr3:uid="{6D77C95E-DD78-44F6-8D6D-0C139A3E7D8A}" uniqueName="22" name="apogee5" queryTableFieldId="22"/>
-    <tableColumn id="23" xr3:uid="{8CC841F1-CC06-499A-8D84-1596D1D21D44}" uniqueName="23" name="apogee6" queryTableFieldId="23"/>
-    <tableColumn id="24" xr3:uid="{8DFB1468-C06D-40CE-B3C2-E24C353802CE}" uniqueName="24" name="apogee7" queryTableFieldId="24"/>
-    <tableColumn id="25" xr3:uid="{56DAB585-6E32-4892-BEA5-32A7CA755F74}" uniqueName="25" name="apogee8" queryTableFieldId="25"/>
-    <tableColumn id="26" xr3:uid="{6B81F15B-A823-408C-8E8D-31DF41E8BD84}" uniqueName="26" name="apogee9" queryTableFieldId="26"/>
-    <tableColumn id="27" xr3:uid="{2FF11B77-3482-4569-89C5-2C6A6621FB28}" uniqueName="27" name="apogee10" queryTableFieldId="27"/>
-    <tableColumn id="28" xr3:uid="{178D91BE-609E-42E7-A21F-45CA15747289}" uniqueName="28" name="apogee11" queryTableFieldId="28"/>
-    <tableColumn id="29" xr3:uid="{6ADDF353-AFCF-4CBB-BEFE-2D8C1910BE4B}" uniqueName="29" name="apogee12" queryTableFieldId="29"/>
+    <tableColumn id="3" xr3:uid="{FB56DFA2-C792-4CE4-B02B-87EFC9B85F6B}" uniqueName="3" name="noseConeShape" queryTableFieldId="3"/>
+    <tableColumn id="4" xr3:uid="{06131C04-BA24-4F0D-AF3B-724D17016671}" uniqueName="4" name="noseConeBluntRadius" queryTableFieldId="4"/>
+    <tableColumn id="5" xr3:uid="{6915BD82-BDC1-41D7-B8A3-302481659DA8}" uniqueName="5" name="noseConeColor" queryTableFieldId="5"/>
+    <tableColumn id="6" xr3:uid="{F38FA88D-02E0-40D5-AC63-CB0CE515693C}" uniqueName="6" name="bodyTubeLength" queryTableFieldId="6"/>
+    <tableColumn id="7" xr3:uid="{C521ED2F-1FC3-4DAB-A9F9-BC51B6DF880D}" uniqueName="7" name="bodyTubeDiameter" queryTableFieldId="7"/>
+    <tableColumn id="8" xr3:uid="{DF644A37-CA42-4F6D-B514-E2DE3DF02CA8}" uniqueName="8" name="bodyTubeColor" queryTableFieldId="8"/>
+    <tableColumn id="9" xr3:uid="{D1CA3669-944B-4A99-BC39-6B262233B95C}" uniqueName="9" name="bodyTubeLength2" queryTableFieldId="9"/>
+    <tableColumn id="10" xr3:uid="{71E57123-8652-4666-BC1D-F74808687DED}" uniqueName="10" name="bodyTubeDiameter2" queryTableFieldId="10"/>
+    <tableColumn id="11" xr3:uid="{9CD28011-0BDA-4F24-A0C9-6B11B5373006}" uniqueName="11" name="bodyTubeColor2" queryTableFieldId="11"/>
+    <tableColumn id="12" xr3:uid="{BA15E9C3-B4CD-4D2B-A5CE-19441D50A3B0}" uniqueName="12" name="finChord" queryTableFieldId="12"/>
+    <tableColumn id="13" xr3:uid="{41E8443E-1025-4CA7-942D-DB72C9332E20}" uniqueName="13" name="finSpan" queryTableFieldId="13"/>
+    <tableColumn id="14" xr3:uid="{1C88E467-9E1D-4275-BCD3-A4F086870034}" uniqueName="14" name="finSweepDistance" queryTableFieldId="14"/>
+    <tableColumn id="15" xr3:uid="{A0A7254A-3F92-44E4-BB66-F7C8FD4E4B96}" uniqueName="15" name="finTipChord" queryTableFieldId="15"/>
+    <tableColumn id="16" xr3:uid="{DA3581A1-3DE9-48D5-9865-AA84BAD78A3C}" uniqueName="16" name="finThickness" queryTableFieldId="16"/>
+    <tableColumn id="17" xr3:uid="{7AACB600-B520-4E15-AF33-7B556520FAD1}" uniqueName="17" name="finLocation" queryTableFieldId="17"/>
+    <tableColumn id="18" xr3:uid="{451CDA72-0A69-401E-88DE-FC3AD6E843ED}" uniqueName="18" name="boosterLength" queryTableFieldId="18"/>
+    <tableColumn id="19" xr3:uid="{9D25066F-609B-46D0-95FD-6CA21A9EEA50}" uniqueName="19" name="boosterDiameter" queryTableFieldId="19"/>
+    <tableColumn id="20" xr3:uid="{1538BFC0-D7C7-4A93-B848-A7F817FE47B3}" uniqueName="20" name="boosterColor" queryTableFieldId="20"/>
+    <tableColumn id="21" xr3:uid="{E2FE5987-0CDC-4B54-B449-7EFEC5EE712B}" uniqueName="21" name="finChord2" queryTableFieldId="21"/>
+    <tableColumn id="22" xr3:uid="{6D77C95E-DD78-44F6-8D6D-0C139A3E7D8A}" uniqueName="22" name="finSpan2" queryTableFieldId="22"/>
+    <tableColumn id="23" xr3:uid="{8CC841F1-CC06-499A-8D84-1596D1D21D44}" uniqueName="23" name="finSweepDistance2" queryTableFieldId="23"/>
+    <tableColumn id="24" xr3:uid="{8DFB1468-C06D-40CE-B3C2-E24C353802CE}" uniqueName="24" name="finTipChord2" queryTableFieldId="24"/>
+    <tableColumn id="25" xr3:uid="{56DAB585-6E32-4892-BEA5-32A7CA755F74}" uniqueName="25" name="finThickness2" queryTableFieldId="25"/>
+    <tableColumn id="26" xr3:uid="{6B81F15B-A823-408C-8E8D-31DF41E8BD84}" uniqueName="26" name="finLocation2" queryTableFieldId="26"/>
+    <tableColumn id="27" xr3:uid="{2FF11B77-3482-4569-89C5-2C6A6621FB28}" uniqueName="27" name="altitude" queryTableFieldId="27"/>
+    <tableColumn id="28" xr3:uid="{178D91BE-609E-42E7-A21F-45CA15747289}" uniqueName="28" name="rodLength" queryTableFieldId="28"/>
+    <tableColumn id="29" xr3:uid="{6ADDF353-AFCF-4CBB-BEFE-2D8C1910BE4B}" uniqueName="29" name="windSpeed" queryTableFieldId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -563,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2BA41CF-4655-44D2-81BA-3AB1895A7CCD}">
   <dimension ref="A1:AC1120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Z13" sqref="Z13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,91 +591,91 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="M1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
       <c r="N1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="O1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="P1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="Q1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="R1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="S1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="T1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="U1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="V1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="W1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="X1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Y1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="Z1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="AA1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="AB1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="AC1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
@@ -686,7 +686,7 @@
         <v>500</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>50</v>
@@ -710,7 +710,7 @@
         <v>40</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="L2">
         <v>60</v>
@@ -737,7 +737,7 @@
         <v>30</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="U2">
         <v>40</v>
@@ -775,7 +775,7 @@
         <v>500</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>50</v>
@@ -799,7 +799,7 @@
         <v>40</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="L3">
         <v>60</v>
@@ -826,7 +826,7 @@
         <v>30</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="U3">
         <v>40</v>
@@ -864,7 +864,7 @@
         <v>500</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>50</v>
@@ -888,7 +888,7 @@
         <v>40</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="L4">
         <v>60</v>
@@ -915,7 +915,7 @@
         <v>30</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="U4">
         <v>40</v>
@@ -953,7 +953,7 @@
         <v>500</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D5">
         <v>50</v>
@@ -977,7 +977,7 @@
         <v>40</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="L5">
         <v>60</v>
@@ -1004,7 +1004,7 @@
         <v>30</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="U5">
         <v>40</v>
@@ -1042,7 +1042,7 @@
         <v>500</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>50</v>
@@ -1066,7 +1066,7 @@
         <v>40</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="L6">
         <v>60</v>
@@ -1093,7 +1093,7 @@
         <v>30</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="U6">
         <v>40</v>
@@ -1131,13 +1131,13 @@
         <v>6.17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="F7">
         <v>17</v>
@@ -1146,7 +1146,7 @@
         <v>6.17</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="I7">
         <v>66</v>
@@ -1155,7 +1155,7 @@
         <v>6.17</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="L7">
         <v>15</v>
@@ -1182,7 +1182,7 @@
         <v>6.17</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="U7">
         <v>15</v>

</xml_diff>